<commit_message>
Final Final folder and most recent edits and corrections as of 11/18/23
</commit_message>
<xml_diff>
--- a/Final Final/Ingestion/Excel Files/IrTotPerEvent.xlsx
+++ b/Final Final/Ingestion/Excel Files/IrTotPerEvent.xlsx
@@ -1,135 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10917"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/allisonadams/My files/Thesis/Microplankton/MicroplanktonAnalysis/Final Final/Ingestion/Excel Files/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33A81C45-0249-B441-B930-D2373CBBF5AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3380" yWindow="500" windowWidth="18460" windowHeight="12540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Allison Adams</author>
-  </authors>
-  <commentList>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{B876C809-3357-3C4E-BCF5-E6049B338849}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Allison Adams:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Total ingestion rate, sum of all taxa groups, pg C per copepod per day</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{0A51AD07-27C6-CC4C-9840-1BE347B53AD0}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Allison Adams:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Total ingestion rate, sum of all taxa groups, µg C per copepod per day</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>event</t>
-  </si>
-  <si>
-    <t>TotalIrpg</t>
-  </si>
-  <si>
-    <t>TotalIRug</t>
-  </si>
-  <si>
-    <t>LSZ2</t>
-  </si>
-  <si>
-    <t>SJR1</t>
-  </si>
-  <si>
-    <t>SJR2</t>
-  </si>
-  <si>
-    <t>WLD2</t>
-  </si>
-  <si>
-    <t>YBP1</t>
-  </si>
-  <si>
-    <t>YBP2</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -144,19 +30,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -179,33 +52,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -243,7 +107,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -277,7 +141,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -312,10 +175,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -488,94 +350,109 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>3</v>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>event</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>TotalIrpg</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>TotalIRug</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>LSZ2</t>
+        </is>
       </c>
       <c r="B2">
-        <v>1719446.3219878459</v>
-      </c>
-      <c r="C2" s="2">
-        <v>1.719446321987846</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>4</v>
+        <v>1719446.157254009</v>
+      </c>
+      <c r="C2">
+        <v>1.719446157254009</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>SJR1</t>
+        </is>
       </c>
       <c r="B3">
-        <v>1439740.6189127739</v>
-      </c>
-      <c r="C3" s="2">
-        <v>1.4397406189127739</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>5</v>
+        <v>1439740.478833043</v>
+      </c>
+      <c r="C3">
+        <v>1.439740478833043</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>SJR2</t>
+        </is>
       </c>
       <c r="B4">
-        <v>199408.8063570619</v>
-      </c>
-      <c r="C4" s="2">
-        <v>0.1994088063570619</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>6</v>
+        <v>199408.7865147504</v>
+      </c>
+      <c r="C4">
+        <v>0.1994087865147504</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>WLD2</t>
+        </is>
       </c>
       <c r="B5">
-        <v>53966.499045764031</v>
-      </c>
-      <c r="C5" s="2">
-        <v>5.3966499045764033E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>7</v>
+        <v>53966.49317578771</v>
+      </c>
+      <c r="C5">
+        <v>0.0539664931757877</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>YBP1</t>
+        </is>
       </c>
       <c r="B6">
-        <v>126637.4853792787</v>
-      </c>
-      <c r="C6" s="2">
-        <v>0.12663748537927871</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>8</v>
+        <v>129209.7753535701</v>
+      </c>
+      <c r="C6">
+        <v>0.1292097753535701</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>YBP2</t>
+        </is>
       </c>
       <c r="B7">
-        <v>5214466.3352452107</v>
-      </c>
-      <c r="C7" s="2">
-        <v>5.214466335245211</v>
+        <v>5214465.807717375</v>
+      </c>
+      <c r="C7">
+        <v>5.214465807717375</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>